<commit_message>
Added new thermometers and barometers found on Zenodo 2021 from Wang
</commit_message>
<xml_diff>
--- a/Benchmarking/olivine_spinel/Supplement_for_Coogan_2014.xlsx
+++ b/Benchmarking/olivine_spinel/Supplement_for_Coogan_2014.xlsx
@@ -5,12 +5,12 @@
   <workbookPr date1904="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://oregonstateuniversity-my.sharepoint.com/personal/wieserp_oregonstate_edu/Documents/Postdoc/PyMME/MyBarometers/Thermobar_outer/Benchmarking/olivine_spinel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\penny\OneDrive - Oregon State University\Postdoc\PyMME\MyBarometers\Thermobar_outer\Benchmarking\olivine_spinel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:40009_{A88A733B-D255-4EEA-8F65-12526E5EFF40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0704EFF8-0E36-4358-936A-3BA46DF4933A}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21E7920C-8A35-473C-B47E-EE140272D664}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="21840" windowHeight="13290" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17790" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Input_for_PTthermobar" sheetId="4" r:id="rId1"/>
@@ -278,9 +278,6 @@
     <t>Cr2O3_Sp</t>
   </si>
   <si>
-    <t>FeO_Sp</t>
-  </si>
-  <si>
     <t>MnO_Sp</t>
   </si>
   <si>
@@ -331,6 +328,9 @@
   <si>
     <t>P2O5_Ol</t>
   </si>
+  <si>
+    <t>FeOt_Sp</t>
+  </si>
 </sst>
 </file>
 
@@ -340,7 +340,7 @@
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
     <numFmt numFmtId="166" formatCode="0.000000"/>
-    <numFmt numFmtId="168" formatCode="0.00000000"/>
+    <numFmt numFmtId="167" formatCode="0.00000000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -396,7 +396,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -454,8 +454,17 @@
     <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -841,8 +850,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AJ31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AC1" workbookViewId="0">
-      <selection activeCell="AJ9" sqref="AJ9"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="X1" sqref="X1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.61328125" defaultRowHeight="12.6" x14ac:dyDescent="0.25"/>
@@ -884,110 +893,110 @@
     <col min="35" max="16384" width="10.61328125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" ht="13.2" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="18" t="s">
+    <row r="1" spans="1:36" s="24" customFormat="1" ht="25.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="22" t="s">
         <v>76</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="D1" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="E1" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="F1" s="18" t="s">
+      <c r="F1" s="22" t="s">
+        <v>88</v>
+      </c>
+      <c r="G1" s="22" t="s">
         <v>89</v>
       </c>
-      <c r="G1" s="18" t="s">
+      <c r="H1" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="I1" s="22" t="s">
         <v>90</v>
       </c>
-      <c r="H1" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="I1" s="18" t="s">
+      <c r="J1" s="22" t="s">
         <v>91</v>
       </c>
-      <c r="J1" s="18" t="s">
+      <c r="K1" s="22" t="s">
         <v>92</v>
       </c>
-      <c r="K1" s="18" t="s">
+      <c r="L1" s="22" t="s">
         <v>93</v>
       </c>
-      <c r="L1" s="18" t="s">
+      <c r="M1" s="22" t="s">
         <v>94</v>
       </c>
-      <c r="M1" s="18" t="s">
+      <c r="N1" s="22" t="s">
         <v>95</v>
       </c>
-      <c r="N1" s="18" t="s">
+      <c r="O1" s="22" t="s">
         <v>96</v>
       </c>
-      <c r="O1" s="18" t="s">
+      <c r="P1" s="22" t="s">
         <v>97</v>
       </c>
-      <c r="P1" s="18" t="s">
+      <c r="Q1" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="R1" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="S1" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="T1" s="22" t="s">
+        <v>77</v>
+      </c>
+      <c r="U1" s="22" t="s">
+        <v>78</v>
+      </c>
+      <c r="V1" s="22" t="s">
+        <v>79</v>
+      </c>
+      <c r="W1" s="22" t="s">
+        <v>80</v>
+      </c>
+      <c r="X1" s="22" t="s">
         <v>98</v>
       </c>
-      <c r="Q1" s="18" t="s">
+      <c r="Y1" s="22" t="s">
+        <v>81</v>
+      </c>
+      <c r="Z1" s="22" t="s">
+        <v>82</v>
+      </c>
+      <c r="AA1" s="22" t="s">
+        <v>83</v>
+      </c>
+      <c r="AB1" s="22" t="s">
+        <v>84</v>
+      </c>
+      <c r="AC1" s="22" t="s">
+        <v>85</v>
+      </c>
+      <c r="AD1" s="22" t="s">
+        <v>86</v>
+      </c>
+      <c r="AE1" s="22" t="s">
+        <v>87</v>
+      </c>
+      <c r="AF1" s="22" t="s">
         <v>58</v>
       </c>
-      <c r="R1" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="S1" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="T1" s="18" t="s">
-        <v>77</v>
-      </c>
-      <c r="U1" s="18" t="s">
-        <v>78</v>
-      </c>
-      <c r="V1" s="18" t="s">
-        <v>79</v>
-      </c>
-      <c r="W1" s="18" t="s">
-        <v>80</v>
-      </c>
-      <c r="X1" s="18" t="s">
-        <v>81</v>
-      </c>
-      <c r="Y1" s="18" t="s">
-        <v>82</v>
-      </c>
-      <c r="Z1" s="18" t="s">
-        <v>83</v>
-      </c>
-      <c r="AA1" s="18" t="s">
-        <v>84</v>
-      </c>
-      <c r="AB1" s="18" t="s">
-        <v>85</v>
-      </c>
-      <c r="AC1" s="18" t="s">
-        <v>86</v>
-      </c>
-      <c r="AD1" s="18" t="s">
-        <v>87</v>
-      </c>
-      <c r="AE1" s="18" t="s">
-        <v>88</v>
-      </c>
-      <c r="AF1" s="18" t="s">
-        <v>58</v>
-      </c>
-      <c r="AG1" s="18" t="s">
+      <c r="AG1" s="22" t="s">
         <v>62</v>
       </c>
-      <c r="AH1" s="19" t="s">
+      <c r="AH1" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="AI1" s="3" t="s">
+      <c r="AI1" s="24" t="s">
         <v>75</v>
       </c>
     </row>

</xml_diff>